<commit_message>
Made user stories revisions
</commit_message>
<xml_diff>
--- a/Documents/Deliverable_1/CSwap_Deliverable_1_ProductBacklog_1.xlsx
+++ b/Documents/Deliverable_1/CSwap_Deliverable_1_ProductBacklog_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/landonthibodeau/git/COS420_Project/Documents/Deliverable_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tonyc\Documents\GitHub\COS420_Project\Documents\Deliverable_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{762FA5E2-8877-E148-92D5-142E666089E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7926D31-03AA-48B1-B226-B9CBCFF34ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="4960" windowWidth="28040" windowHeight="17440" xr2:uid="{0464AEB8-671C-F246-822E-B13A3778F0CA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{0464AEB8-671C-F246-822E-B13A3778F0CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,32 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Story</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Story Priority</t>
+  </si>
+  <si>
+    <t>Story Status</t>
+  </si>
+  <si>
+    <t>Story Points</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -43,13 +66,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -61,13 +97,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -380,12 +419,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D71E41-7656-BB48-93A1-08AE0A3374DC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="4" max="4" width="26.4140625" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated user stories and started adding to the product backlog
</commit_message>
<xml_diff>
--- a/Documents/Deliverable_1/CSwap_Deliverable_1_ProductBacklog_1.xlsx
+++ b/Documents/Deliverable_1/CSwap_Deliverable_1_ProductBacklog_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tonyc\Documents\GitHub\COS420_Project\Documents\Deliverable_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7926D31-03AA-48B1-B226-B9CBCFF34ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC6303F-64F8-479F-B352-AD742CEED17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{0464AEB8-671C-F246-822E-B13A3778F0CA}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="28800" windowHeight="15460" xr2:uid="{0464AEB8-671C-F246-822E-B13A3778F0CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -52,13 +52,43 @@
   </si>
   <si>
     <t>Story Points</t>
+  </si>
+  <si>
+    <t>As a new student, I want to be able to navigate over to the book section so that I can buy textbooks for my classes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a seller, I want to be able to sell my items in my local area so that relevant buyers can find my items.  </t>
+  </si>
+  <si>
+    <t>As an unauthorized user I want create a new account so I can buy and sell items.</t>
+  </si>
+  <si>
+    <t>As an unauthorized user I want to login my account so that I can access my info.</t>
+  </si>
+  <si>
+    <t>As an authorized user I want to logout of my account so that a stranger cannot use my account</t>
+  </si>
+  <si>
+    <t>As a user I want to be able to add an item to the list</t>
+  </si>
+  <si>
+    <t>As an unauthorized user I want to use my google account so that I can use one of my own existing accounts.</t>
+  </si>
+  <si>
+    <t>As an unauthorized user I want to use my Facebook account so that I can use one of my own existing accounts.</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -73,8 +103,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -87,8 +130,13 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -96,17 +144,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -422,12 +490,12 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="71.4140625" customWidth="1"/>
     <col min="3" max="3" width="22.83203125" customWidth="1"/>
     <col min="4" max="4" width="26.4140625" customWidth="1"/>
     <col min="5" max="5" width="27.6640625" customWidth="1"/>
@@ -458,48 +526,162 @@
       <c r="A2">
         <v>0</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E10" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Modified Product Backlog for sprint 1
</commit_message>
<xml_diff>
--- a/Documents/Deliverable_1/CSwap_Deliverable_1_ProductBacklog_1.xlsx
+++ b/Documents/Deliverable_1/CSwap_Deliverable_1_ProductBacklog_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tonyc\Documents\GitHub\COS420_Project\Documents\Deliverable_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/landonthibodeau/git/COS420_Project/Documents/Deliverable_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC6303F-64F8-479F-B352-AD742CEED17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520E7682-A6AC-A44E-9023-242B8A534456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="28800" windowHeight="15460" xr2:uid="{0464AEB8-671C-F246-822E-B13A3778F0CA}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="20560" windowHeight="25700" xr2:uid="{0464AEB8-671C-F246-822E-B13A3778F0CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,17 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Story</t>
-  </si>
-  <si>
-    <t>Sprint</t>
-  </si>
-  <si>
     <t>Story Priority</t>
   </si>
   <si>
@@ -69,9 +63,6 @@
     <t>As an authorized user I want to logout of my account so that a stranger cannot use my account</t>
   </si>
   <si>
-    <t>As a user I want to be able to add an item to the list</t>
-  </si>
-  <si>
     <t>As an unauthorized user I want to use my google account so that I can use one of my own existing accounts.</t>
   </si>
   <si>
@@ -82,13 +73,28 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>User Story</t>
+  </si>
+  <si>
+    <t>Sprint Number</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>As a student looking for an apartment, I want to sort the apartment offerings by price so that I can find an apartment that I can easily afford</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -104,13 +110,51 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -163,14 +207,31 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -487,209 +548,212 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D71E41-7656-BB48-93A1-08AE0A3374DC}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="71.4140625" customWidth="1"/>
+    <col min="2" max="2" width="71.33203125" customWidth="1"/>
     <col min="3" max="3" width="22.83203125" customWidth="1"/>
-    <col min="4" max="4" width="26.4140625" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
     <col min="5" max="5" width="27.6640625" customWidth="1"/>
     <col min="6" max="6" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="42" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="42" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="42" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="43" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="65" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="44" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="44" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="68" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="27" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>7</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>6</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>10</v>
-      </c>
+      <c r="B11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added more user stories to Product backlog
</commit_message>
<xml_diff>
--- a/Documents/Deliverable_1/CSwap_Deliverable_1_ProductBacklog_1.xlsx
+++ b/Documents/Deliverable_1/CSwap_Deliverable_1_ProductBacklog_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/landonthibodeau/git/COS420_Project/Documents/Deliverable_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tonyc\Documents\GitHub\COS420_Project\Documents\Deliverable_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17746E62-3164-D243-B2E3-20EA4752DF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B671045B-7D50-40EA-81CE-C5D1B63546F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="20560" windowHeight="25700" xr2:uid="{0464AEB8-671C-F246-822E-B13A3778F0CA}"/>
+    <workbookView xWindow="6380" yWindow="2000" windowWidth="28800" windowHeight="15460" xr2:uid="{0464AEB8-671C-F246-822E-B13A3778F0CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -84,10 +84,64 @@
     <t>H</t>
   </si>
   <si>
-    <t>As a student looking for an apartment, I want to sort the apartment offerings by price so that I can find an apartment that I can easily afford</t>
-  </si>
-  <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>As a student looking for an apartment, I want to sort the apartment offerings by price so that I can find an apartment that I can afford easily.</t>
+  </si>
+  <si>
+    <t>As a landlord, I want to advertise one of my apartments on the apartment section so that students can find and rent my apartment.</t>
+  </si>
+  <si>
+    <t>As a student looking to sell my textbook, I want to list last year's textbooks for sale so that I can get some money for them.</t>
+  </si>
+  <si>
+    <t>As a student looking to sell my textbook, I want a list of how much users paid for this textbook last semester so I can make money.</t>
+  </si>
+  <si>
+    <t>As a student selling items, I want to edit the tags on my listing so that they can get better exposure.</t>
+  </si>
+  <si>
+    <t>As a student looking for furniture, I want to use CSwap and navigate to the furniture section so that I can find furniture for my apartment.</t>
+  </si>
+  <si>
+    <t>As a student looking for furniture, I want to sort the furniture section so that I can find only what I need.</t>
+  </si>
+  <si>
+    <t>As a seller, I want to list my calculator for sale under the electronics section so that other students can buy it.</t>
+  </si>
+  <si>
+    <t>As a user, I want a profile so that I can see what the person I am selling to looks like.</t>
+  </si>
+  <si>
+    <t>As a seller, I want to add new photos to my listing so that my listing is more attractive.</t>
+  </si>
+  <si>
+    <t>As a user, I want to delete my account so that I am no longer active on the app.</t>
+  </si>
+  <si>
+    <t>As a seller, I want to change the description of my listing so that It’s available for both pick up and for delivery.</t>
+  </si>
+  <si>
+    <t>As a landlord, I want to be able to list my apartment under multiple colleges so that my apartment will be seen by people in the area.</t>
+  </si>
+  <si>
+    <t>As a seller, I want to be able to see all the items I am currently selling so that I know from organizational purposes.</t>
+  </si>
+  <si>
+    <t>As a seller, I want to see how long my listing has been on the website so that I can determine if I need to make a change to the listing.</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to give ratings to a seller so that I can help provide useful feedback on the buying process.</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to see my recently viewed listings so that I can go back to view listings I previously visited.</t>
+  </si>
+  <si>
+    <t>As a student, I want to be able to have a book condition tag so that I can sell my high-quality books for more money.</t>
+  </si>
+  <si>
+    <t>As a student user, I want to filter out listings above a price range so I don't only see listings I can't afford.</t>
   </si>
 </sst>
 </file>
@@ -209,7 +263,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -231,6 +285,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -548,13 +608,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D71E41-7656-BB48-93A1-08AE0A3374DC}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="71.33203125" customWidth="1"/>
     <col min="3" max="3" width="22.83203125" customWidth="1"/>
@@ -563,7 +623,7 @@
     <col min="6" max="6" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,7 +643,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="40" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -603,7 +663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="42" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="40" x14ac:dyDescent="0.4">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -623,7 +683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="42" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="40" x14ac:dyDescent="0.4">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -643,7 +703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="40.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -663,7 +723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="65" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="41" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -683,7 +743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="44" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="41" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -703,7 +763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="44" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="41" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -723,18 +783,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="68" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="61" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>16</v>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="C9" s="5">
         <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>12</v>
@@ -743,17 +803,470 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="27" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="61" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5">
+        <v>3</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="61" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="5">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="61" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="5">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="41" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="5">
+        <v>6</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="61" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="5">
+        <v>7</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="41" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="5">
+        <v>8</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="41" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="5">
+        <v>9</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="41" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="5">
+        <v>10</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="41" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="5">
+        <v>11</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="41" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="5">
+        <v>12</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="41" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="5">
+        <v>13</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="61" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="5">
+        <v>14</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="5">
+        <v>15</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="63" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="5">
+        <v>16</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="44" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="5">
+        <v>17</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="50.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="5">
+        <v>18</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="5">
+        <v>19</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="41" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="5">
+        <v>20</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="26.5" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" ht="26" x14ac:dyDescent="0.5">
+      <c r="A29" s="2"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" ht="26" x14ac:dyDescent="0.5">
+      <c r="A30" s="2"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" ht="26" x14ac:dyDescent="0.5">
+      <c r="A31" s="2"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" ht="26" x14ac:dyDescent="0.5">
+      <c r="A32" s="2"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" ht="26" x14ac:dyDescent="0.5">
+      <c r="A33" s="2"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" ht="26" x14ac:dyDescent="0.5">
+      <c r="A34" s="2"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:6" ht="26" x14ac:dyDescent="0.5">
+      <c r="A35" s="2"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:6" ht="26" x14ac:dyDescent="0.5">
+      <c r="A36" s="2"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" ht="26" x14ac:dyDescent="0.5">
+      <c r="A37" s="2"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:6" ht="26" x14ac:dyDescent="0.5">
+      <c r="A38" s="2"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" ht="26" x14ac:dyDescent="0.5">
+      <c r="A39" s="2"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.5">
+      <c r="A40" s="2"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:6" ht="26" x14ac:dyDescent="0.5">
+      <c r="A41" s="2"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" ht="26" x14ac:dyDescent="0.5">
+      <c r="A42" s="2"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="F42" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>